<commit_message>
Code Checkin as part NI Module testing for release PayrollP2.1
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite MonthlyCatJ201819.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite MonthlyCatJ201819.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="3" windowHeight="4455" windowWidth="14340" xWindow="390" yWindow="90"/>
+    <workbookView xWindow="390" yWindow="90" windowWidth="14340" windowHeight="4455" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="first" r:id="rId1" sheetId="1"/>
-    <sheet name="NIMonthlyCat_J" r:id="rId2" sheetId="2"/>
-    <sheet name="ProcessPayrollForNIMonthly" r:id="rId3" sheetId="4"/>
-    <sheet name="TestReports" r:id="rId4" sheetId="5"/>
+    <sheet name="first" sheetId="1" r:id="rId1"/>
+    <sheet name="NIMonthlyCat_J" sheetId="2" r:id="rId2"/>
+    <sheet name="ProcessPayrollForNIMonthly" sheetId="4" r:id="rId3"/>
+    <sheet name="TestReports" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="63">
   <si>
     <t>TC</t>
   </si>
@@ -211,16 +211,12 @@
   </si>
   <si>
     <t>F:\\Automation_TestResults\\Payroll_Tax_NI_Directors_TestReports 201819\\201819 Payroll National Insurance calculation Test result.xlsx</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Admin\\git\\XCDHR_Payroll\\Salesforce_Core_Framework\\TestOutPutResultFolder\\201819 Payroll National Insurance calculation Test result.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -268,48 +264,48 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -326,10 +322,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -364,7 +360,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -416,7 +412,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -521,7 +517,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -530,13 +526,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -546,7 +542,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -555,7 +551,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -564,7 +560,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -574,12 +570,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -610,7 +606,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -629,7 +625,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -641,7 +637,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -650,10 +646,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="48.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="33.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
+    <col min="1" max="1" width="48.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="33.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -684,7 +680,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
@@ -698,7 +694,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" ht="45" r="4" s="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
@@ -726,7 +722,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" ht="30" r="6" s="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -740,7 +736,7 @@
         <v>7</v>
       </c>
     </row>
-    <row ht="75" r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -755,13 +751,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -770,12 +766,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="42.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="80.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="4" width="15.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="42" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="80.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -962,16 +958,16 @@
       <c r="H10" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="C2:C10"/>
+    <ignoredError sqref="C2:C10" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -980,19 +976,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="51.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="40.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="32.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="42.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="55.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="1" max="1" width="51.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="40" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="32.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="42.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="55.28515625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="35.450000000000003" r="1" s="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="7" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>25</v>
       </c>
@@ -1033,7 +1029,7 @@
         <v>11</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="50.25" r="2" s="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="9" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>47</v>
       </c>
@@ -1068,7 +1064,7 @@
         <v>6</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="35.450000000000003" r="3" s="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="7" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>47</v>
       </c>
@@ -1105,7 +1101,7 @@
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="35.450000000000003" r="4" s="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="7" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>47</v>
       </c>
@@ -1142,7 +1138,7 @@
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="35.450000000000003" r="5" s="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="7" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>47</v>
       </c>
@@ -1179,7 +1175,7 @@
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="35.450000000000003" r="6" s="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="7" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>47</v>
       </c>
@@ -1216,7 +1212,7 @@
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="35.450000000000003" r="7" s="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="7" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>47</v>
       </c>
@@ -1253,7 +1249,7 @@
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="35.450000000000003" r="8" s="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="7" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>47</v>
       </c>
@@ -1290,7 +1286,7 @@
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="35.450000000000003" r="9" s="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="10" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>47</v>
       </c>
@@ -1327,7 +1323,7 @@
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="45.75" r="10" s="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="10" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>47</v>
       </c>
@@ -1366,39 +1362,39 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A3:A10"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink ref="A3:A10" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="50.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="33.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="44.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="55.85546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="23.7109375" collapsed="false"/>
-    <col min="15" max="15" customWidth="true" width="55.28515625" collapsed="false"/>
+    <col min="1" max="1" width="50.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="44.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="55.85546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.42578125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="23.7109375" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="55.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="34.15" r="1" s="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="7" customFormat="1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>25</v>
       </c>
@@ -1442,7 +1438,7 @@
         <v>11</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="51" r="2" s="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="9" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>47</v>
       </c>
@@ -1464,8 +1460,8 @@
       <c r="G2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>63</v>
+      <c r="H2" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>38</v>
@@ -1485,10 +1481,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A2"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="A2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>